<commit_message>
Changes for updating issue
</commit_message>
<xml_diff>
--- a/docs/Jira BUG Matrix.xlsx
+++ b/docs/Jira BUG Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s.kumar\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SourceCode\JiraTesterPro\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="37">
   <si>
     <t>New</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Deferred</t>
   </si>
   <si>
-    <t>DEFERRED</t>
-  </si>
-  <si>
     <t>Stop Progress</t>
   </si>
   <si>
@@ -132,13 +129,19 @@
   </si>
   <si>
     <t>ED</t>
+  </si>
+  <si>
+    <t>IssueType</t>
+  </si>
+  <si>
+    <t>Bug</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,13 +159,6 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -218,12 +214,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -236,13 +231,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -525,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,262 +540,262 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>35</v>
       </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="3" spans="1:12" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="F4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I3" s="7" t="s">
+      <c r="L4" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>3</v>
+      <c r="A5" s="5" t="s">
+        <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>23</v>
+        <v>14</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>4</v>
+      <c r="A6" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>5</v>
+      <c r="A7" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K8" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L9" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for format of test result output
</commit_message>
<xml_diff>
--- a/docs/Jira BUG Matrix.xlsx
+++ b/docs/Jira BUG Matrix.xlsx
@@ -523,22 +523,22 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="46" customWidth="1"/>
-    <col min="2" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="2" max="5" width="20.7265625" customWidth="1"/>
+    <col min="6" max="7" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="19.85546875" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.81640625" customWidth="1"/>
+    <col min="12" max="12" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -546,7 +546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -554,7 +554,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="139.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
@@ -570,7 +570,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -608,7 +608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -646,7 +646,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -684,7 +684,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
@@ -722,7 +722,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>5</v>
       </c>
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>11</v>
       </c>

</xml_diff>